<commit_message>
First release BLT1 test item data
</commit_message>
<xml_diff>
--- a/0WM_BLT1/Process/0WM_BLT1_DVT.xlsx
+++ b/0WM_BLT1/Process/0WM_BLT1_DVT.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="185">
   <si>
     <t>ID</t>
   </si>
@@ -149,69 +149,6 @@
     <t>B2LDW</t>
   </si>
   <si>
-    <t>HDMI_Status</t>
-  </si>
-  <si>
-    <t>VeriCBIOP</t>
-  </si>
-  <si>
-    <t>VeriIMU</t>
-  </si>
-  <si>
-    <t>VeriIMUINTs</t>
-  </si>
-  <si>
-    <t>VeriUBI2C</t>
-  </si>
-  <si>
-    <t>VeriUSB2</t>
-  </si>
-  <si>
-    <t>WrPCBASN</t>
-  </si>
-  <si>
-    <t>ChkBiosVer</t>
-  </si>
-  <si>
-    <t>ChkImgVer</t>
-  </si>
-  <si>
-    <t>ChkPCBASN</t>
-  </si>
-  <si>
-    <t>ChkStoInf</t>
-  </si>
-  <si>
-    <t>ChkWIFI5G</t>
-  </si>
-  <si>
-    <t>ChkWIFI2G</t>
-  </si>
-  <si>
-    <t>ChkMBINT</t>
-  </si>
-  <si>
-    <t>ChkBTP</t>
-  </si>
-  <si>
-    <t>ChkBTMAC</t>
-  </si>
-  <si>
-    <t>ChkWIFIMAC</t>
-  </si>
-  <si>
-    <t>VeriLB1I2C</t>
-  </si>
-  <si>
-    <t>VeriLB2I2C</t>
-  </si>
-  <si>
-    <t>VeriUART</t>
-  </si>
-  <si>
-    <t>ChkWIFI2GND</t>
-  </si>
-  <si>
     <t>P1V5V</t>
   </si>
   <si>
@@ -239,144 +176,12 @@
     <t>START</t>
   </si>
   <si>
-    <t>Reset_Button</t>
-  </si>
-  <si>
     <t>C:\TestProgram\0WM\0WM_BLT1\Test_start.bat</t>
   </si>
   <si>
     <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_start_log.bat</t>
   </si>
   <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_Reset_Button.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_Reset_Button_log.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_HDMI_Status.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_HDMI_Status_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_WrPCBASN.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_WrPCBASN_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_ChkBTP.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_ChkBTP_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_ChkMBINT.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_ChkWIFI2G.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_ChkWIFI2G_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_ChkWIFI2GND.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_ChkWIFI2GND_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_ChkWIFI5G.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_ChkWIFI5G_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_ChkBiosVer.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_ChkBiosVer_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_ChkImgVer.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_ChkImgVer_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_ChkPCBASN.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_ChkPCBASN_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_ChkStoInf.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_ChkStoInf_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_ChkBTMAC.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_ChkBTMAC_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_ChkWIFIMAC.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_ChkWIFIMAC_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_VeriCBIOP.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_VeriCBIOP_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_VeriIMU.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_VeriIMU_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_VeriIMUINTs.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_VeriIMUINTs_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_VeriLB1I2C.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_VeriLB1I2C_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_VeriLB2I2C.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_VeriLB2I2C_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_VeriUBI2C.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_VeriUBI2C_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_VeriUSB2.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_VeriUSB2_CheckLog.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_VeriUART.bat</t>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_VeriUART_CheckLog.bat</t>
-  </si>
-  <si>
     <t>I2C_PowerMonitor_INA230</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -389,10 +194,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_ChkMBINT_CheckLog.bat</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>I2C_TempSensor_TMP108</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -438,6 +239,468 @@
   </si>
   <si>
     <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_I2C_EEPROM_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>I2C_BusSwitch</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_I2C_BusSwitch.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_I2C_BusSwitch_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WriteMAC_I219</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_WriteMAC_I219.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_WriteMAC_I219_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckMAC_I219</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckMAC_I219.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckMAC_I219_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WriteMAC_WIFI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_WriteMAC_WIFI.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_WriteMAC_WIFI_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckMAC_WIFI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckMAC_WIFI.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckMAC_WIFI_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckMAC_BT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckMAC_BT.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckMAC_BT_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WriteMAC_BT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_WriteMAC_BT.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_WriteMAC_BT_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WriteMAC_WGI210</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_WriteMAC_WGI210.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_WriteMAC_WGI210_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckMAC_WGI210</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckMAC_WGI210.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckMAC_WGI210_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WriteMAC_FPGA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_WriteMAC_FPGA.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_WriteMAC_FPGA_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckMAC_FPGA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckMAC_FPGA.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckMAC_FPGA_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WriteProductName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_WriteProductName.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_WriteProductName_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckProductName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckProductName.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckProductName_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WriteProductVersion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_WriteProductVersion.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_WriteProductVersion_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckProductVersion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckProductVersion.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckProductVersion_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WriteProductUUID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_WriteProductUUID.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_WriteProductUUID_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckProductUUID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckProductUUID.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckProductUUID_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckImageVer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckImageVer.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckImageVer_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckBIOSVer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckBIOSVer.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckBIOSVer_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckUSBTypeCFWVer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckUSBTypeCFWVer.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckUSBTypeCFWVer_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckOROMVer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckOROMVer.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckOROMVer_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckCPLDVer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_CheckCPLDVer.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_CheckCPLDVer_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP_Port1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_DP_Port1.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_DP_Port1_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP_HDMI_Port1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_DP_HDMI_Port1.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_DP_HDMI_Port1_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP_Port2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_DP_Port2.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_DP_Port2_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP_HDMI_Port2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_DP_HDMI_Port2.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_DP_HDMI_Port2_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_TypeA_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_USB_TypeA_1.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_USB_TypeA_1_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_TypeA_2_RJ45_2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_USB_TypeA_2_RJ45_2.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_USB_TypeA_2_RJ45_2_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_TypeC_1_RJ45_1</t>
+  </si>
+  <si>
+    <t>USB_TypeC_1_RJ45_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_USB_TypeC_1_RJ45_1.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_USB_TypeC_1_RJ45_1_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_TypeC_DP_1</t>
+  </si>
+  <si>
+    <t>USB_TypeC_DP_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_USB_TypeC_DP_1.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_USB_TypeC_DP_1_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_TypeC_PD_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_USB_TypeC_PD_1.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_USB_TypeC_PD_1_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_TypeC_2_RJ45_1</t>
+  </si>
+  <si>
+    <t>USB_TypeC_2_RJ45_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_USB_TypeC_2_RJ45_1.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_USB_TypeC_2_RJ45_1_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_TypeC_DP_2</t>
+  </si>
+  <si>
+    <t>USB_TypeC_DP_2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_USB_TypeC_DP_2.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_USB_TypeC_DP_2_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB_TypeC_PD_2</t>
+  </si>
+  <si>
+    <t>USB_TypeC_PD_2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_USB_TypeC_PD_2.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_USB_TypeC_PD_2_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gizmo_Port</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_Gizmo_Port.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_Gizmo_Port_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RJ45_Loopback_Port3_4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_RJ45_Loopback_Port3_4.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_RJ45_Loopback_Port3_4_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>LED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_LED.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_LED_CheckLog.bat</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -829,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -920,27 +1183,27 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>23</v>
@@ -954,25 +1217,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>118</v>
+        <v>53</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>118</v>
+        <v>53</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="R3" s="3">
         <v>2</v>
@@ -983,22 +1246,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>123</v>
+        <v>57</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>124</v>
+        <v>58</v>
       </c>
       <c r="M4" s="3">
         <v>4</v>
@@ -1012,22 +1275,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>125</v>
+        <v>59</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>125</v>
+        <v>59</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>126</v>
+        <v>60</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>127</v>
+        <v>61</v>
       </c>
       <c r="M5" s="3">
         <v>4</v>
@@ -1041,22 +1304,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>128</v>
+        <v>62</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>128</v>
+        <v>62</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>129</v>
+        <v>63</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>130</v>
+        <v>64</v>
       </c>
       <c r="M6" s="3">
         <v>4</v>
@@ -1070,22 +1333,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>132</v>
+        <v>66</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>133</v>
+        <v>67</v>
       </c>
       <c r="M7" s="3">
         <v>4</v>
@@ -1099,22 +1362,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="K8" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M8" s="3">
         <v>4</v>
@@ -1128,22 +1391,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="M9" s="2">
         <v>4</v>
@@ -1157,22 +1420,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>23</v>
@@ -1186,22 +1449,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>23</v>
@@ -1215,22 +1478,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>23</v>
@@ -1244,22 +1507,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="M13" s="2">
         <v>8</v>
@@ -1273,22 +1536,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M14" s="2">
         <v>8</v>
@@ -1302,22 +1565,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>27</v>
@@ -1331,22 +1594,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="M16" s="2">
         <v>8</v>
@@ -1360,22 +1623,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="M17" s="2">
         <v>8</v>
@@ -1389,22 +1652,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>31</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="M18" s="2">
         <v>8</v>
@@ -1418,22 +1681,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>32</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>23</v>
@@ -1447,22 +1710,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>33</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="M20" s="2">
         <v>8</v>
@@ -1476,22 +1739,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>33</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="M21" s="2">
         <v>8</v>
@@ -1505,22 +1768,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>34</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>23</v>
@@ -1534,22 +1797,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>35</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>23</v>
@@ -1563,22 +1826,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>36</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>23</v>
@@ -1592,22 +1855,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>37</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>23</v>
@@ -1621,22 +1884,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>37</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>23</v>
@@ -1650,22 +1913,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>38</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>23</v>
@@ -1679,22 +1942,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>47</v>
+        <v>128</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>47</v>
+        <v>128</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>39</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>23</v>
@@ -1708,28 +1971,463 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>40</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="R29" s="3">
         <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="M32" s="3">
+        <v>4</v>
+      </c>
+      <c r="R32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="M33" s="3">
+        <v>4</v>
+      </c>
+      <c r="R33" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="M34" s="3">
+        <v>4</v>
+      </c>
+      <c r="R34" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="M35" s="3">
+        <v>4</v>
+      </c>
+      <c r="R35" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="M36" s="3">
+        <v>4</v>
+      </c>
+      <c r="R36" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="M37" s="2">
+        <v>4</v>
+      </c>
+      <c r="R37" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A38" s="3">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R38" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A39" s="3">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R39" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A40" s="3">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R40" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A41" s="3">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="M41" s="2">
+        <v>8</v>
+      </c>
+      <c r="R41" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A42" s="3">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="M42" s="2">
+        <v>8</v>
+      </c>
+      <c r="R42" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A43" s="3">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R43" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A44" s="3">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="M44" s="2">
+        <v>8</v>
+      </c>
+      <c r="R44" s="3">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change LED test item name
</commit_message>
<xml_diff>
--- a/0WM_BLT1/Process/0WM_BLT1_DVT.xlsx
+++ b/0WM_BLT1/Process/0WM_BLT1_DVT.xlsx
@@ -686,18 +686,19 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>LED</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_LED.bat</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_LED_CheckLog.bat</t>
+    <t>LED1to6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED1to6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_LED1to6.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_LED1to6_CheckLog.bat</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1091,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2403,13 +2404,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Update test script from test plan
</commit_message>
<xml_diff>
--- a/0WM_BLT1/Process/0WM_BLT1_DVT.xlsx
+++ b/0WM_BLT1/Process/0WM_BLT1_DVT.xlsx
@@ -203,18 +203,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>I2C_AccelerometerSensor_ISM303DAC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\Test_I2C_AccelerometerSensor_ISM303DAC.bat</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_I2C_AccelerometerSensor_ISM303DAC_CheckLog.bat</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>I2C_ShifterRetimer_SN65DP159</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -699,6 +687,18 @@
   </si>
   <si>
     <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_LED1to6_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>I2C_AccelSensor_ISM303DAC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\Test_I2C_AccelSensor_ISM303DAC.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT1\log\Test_I2C_AccelSensor_ISM303DAC_CheckLog.bat</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1092,14 +1092,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="37.125" style="2" customWidth="1"/>
     <col min="3" max="3" width="4.25" style="2" customWidth="1"/>
     <col min="4" max="4" width="5.25" style="2" customWidth="1"/>
     <col min="5" max="5" width="5" style="2" customWidth="1"/>
@@ -1273,22 +1273,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>181</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>58</v>
+        <v>181</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>59</v>
+        <v>182</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>60</v>
+        <v>183</v>
       </c>
       <c r="M5" s="3">
         <v>8</v>
@@ -1302,22 +1302,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M6" s="3">
         <v>8</v>
@@ -1331,22 +1331,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>46</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M7" s="3">
         <v>8</v>
@@ -1360,22 +1360,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>47</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M8" s="3">
         <v>8</v>
@@ -1389,22 +1389,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M9" s="3">
         <v>8</v>
@@ -1418,22 +1418,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M10" s="2">
         <v>8</v>
@@ -1447,22 +1447,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="M11" s="2">
         <v>8</v>
@@ -1476,22 +1476,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M12" s="2">
         <v>8</v>
@@ -1505,22 +1505,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M13" s="2">
         <v>8</v>
@@ -1534,22 +1534,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M14" s="2">
         <v>8</v>
@@ -1563,22 +1563,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>27</v>
@@ -1592,22 +1592,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="M16" s="2">
         <v>8</v>
@@ -1621,22 +1621,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="M17" s="2">
         <v>8</v>
@@ -1650,22 +1650,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>31</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M18" s="2">
         <v>8</v>
@@ -1679,22 +1679,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>32</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M19" s="2">
         <v>8</v>
@@ -1708,22 +1708,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>33</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="M20" s="2">
         <v>8</v>
@@ -1737,22 +1737,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>33</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="M21" s="2">
         <v>8</v>
@@ -1766,22 +1766,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>34</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="M22" s="2">
         <v>8</v>
@@ -1795,22 +1795,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>35</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M23" s="2">
         <v>8</v>
@@ -1824,22 +1824,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>36</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="M24" s="2">
         <v>8</v>
@@ -1853,22 +1853,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>37</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="M25" s="2">
         <v>8</v>
@@ -1882,22 +1882,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>37</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="M26" s="2">
         <v>4</v>
@@ -1911,22 +1911,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>38</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M27" s="2">
         <v>4</v>
@@ -1940,22 +1940,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>39</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="M28" s="2">
         <v>4</v>
@@ -1969,22 +1969,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>40</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="M29" s="2">
         <v>4</v>
@@ -1998,22 +1998,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>49</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="M30" s="3" t="s">
         <v>23</v>
@@ -2027,22 +2027,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>42</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M31" s="3">
         <v>4</v>
@@ -2056,22 +2056,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>43</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M32" s="3">
         <v>4</v>
@@ -2085,22 +2085,22 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="M33" s="3">
         <v>4</v>
@@ -2114,22 +2114,22 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="M34" s="3">
         <v>4</v>
@@ -2143,22 +2143,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>46</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M35" s="3">
         <v>4</v>
@@ -2172,22 +2172,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>47</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="M36" s="3">
         <v>4</v>
@@ -2201,22 +2201,22 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="M37" s="2">
         <v>4</v>
@@ -2230,22 +2230,22 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>23</v>
@@ -2259,22 +2259,22 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>23</v>
@@ -2288,22 +2288,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>24</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>23</v>
@@ -2317,22 +2317,22 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="M41" s="2">
         <v>4</v>
@@ -2346,22 +2346,22 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M42" s="2">
         <v>4</v>
@@ -2375,22 +2375,22 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="M43" s="2">
         <v>4</v>
@@ -2404,22 +2404,22 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>29</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="M44" s="2">
         <v>4</v>

</xml_diff>